<commit_message>
Added RSVPLinkId (PK) to Table RSVPLink
Updated WeddingID (PK) to WeddingID (FK)
Updated PersonID (PK) to PersonID (FK)
</commit_message>
<xml_diff>
--- a/Wedding Builder Data Model.xlsx
+++ b/Wedding Builder Data Model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\435TeamProject\WeddingSiteBuilderSQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephanie\Documents\_UM Dearborn - CIS 435 Web Technology\Group Project\Data Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="116">
   <si>
     <t>Column Name</t>
   </si>
@@ -403,6 +403,9 @@
       </rPr>
       <t xml:space="preserve"> datetime</t>
     </r>
+  </si>
+  <si>
+    <t>RSVPLinkId (PK)</t>
   </si>
 </sst>
 </file>
@@ -704,6 +707,12 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -711,12 +720,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1003,7 +1006,7 @@
   <dimension ref="B2:K77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46:K46"/>
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,18 +1028,18 @@
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24"/>
-      <c r="H3" s="22" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
+      <c r="H3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="24"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="26"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -1170,7 +1173,7 @@
       <c r="B9" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="23" t="s">
         <v>114</v>
       </c>
       <c r="D9" s="12" t="s">
@@ -1182,7 +1185,7 @@
       <c r="H9" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="I9" s="23" t="s">
         <v>114</v>
       </c>
       <c r="J9" s="12" t="s">
@@ -1200,18 +1203,18 @@
       <c r="K10" s="14"/>
     </row>
     <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
-      <c r="H11" s="22" t="s">
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="26"/>
+      <c r="H11" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="24"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
@@ -1501,7 +1504,7 @@
       <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="22" t="s">
         <v>113</v>
       </c>
       <c r="D23" s="11" t="s">
@@ -1553,7 +1556,7 @@
       <c r="B25" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="23" t="s">
         <v>114</v>
       </c>
       <c r="D25" s="12" t="s">
@@ -1604,12 +1607,12 @@
       </c>
     </row>
     <row r="28" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="24"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="26"/>
       <c r="H28" s="2" t="s">
         <v>17</v>
       </c>
@@ -1665,7 +1668,7 @@
       <c r="H30" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="I30" s="26" t="s">
+      <c r="I30" s="23" t="s">
         <v>114</v>
       </c>
       <c r="J30" s="12" t="s">
@@ -1733,12 +1736,12 @@
       <c r="E34" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="22" t="s">
+      <c r="H34" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
-      <c r="K34" s="24"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="26"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
@@ -1780,7 +1783,7 @@
         <v>39</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="I36" s="11" t="s">
         <v>79</v>
@@ -1806,7 +1809,7 @@
         <v>68</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="I37" s="11" t="s">
         <v>79</v>
@@ -1815,10 +1818,10 @@
         <v>26</v>
       </c>
       <c r="K37" s="9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
         <v>11</v>
       </c>
@@ -1831,20 +1834,20 @@
       <c r="E38" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="H38" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>58</v>
+      <c r="H38" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="J38" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K38" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>109</v>
       </c>
@@ -1857,17 +1860,17 @@
       <c r="E39" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I39" s="25" t="s">
-        <v>113</v>
+      <c r="H39" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="J39" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K39" s="9" t="s">
-        <v>64</v>
+      <c r="K39" s="16" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
@@ -1883,20 +1886,20 @@
       <c r="E40" s="21">
         <v>42170.583333333336</v>
       </c>
-      <c r="H40" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>80</v>
+      <c r="H40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40" s="22" t="s">
+        <v>113</v>
       </c>
       <c r="J40" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K40" s="21">
-        <v>42170.583333333336</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K40" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
         <v>104</v>
       </c>
@@ -1909,24 +1912,24 @@
       <c r="E41" s="21">
         <v>42170.583333333336</v>
       </c>
-      <c r="H41" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="I41" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="J41" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K41" s="10" t="s">
-        <v>106</v>
+      <c r="H41" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K41" s="21">
+        <v>42170.583333333336</v>
       </c>
     </row>
     <row r="42" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C42" s="26" t="s">
+      <c r="C42" s="23" t="s">
         <v>114</v>
       </c>
       <c r="D42" s="12" t="s">
@@ -1935,15 +1938,27 @@
       <c r="E42" s="10" t="s">
         <v>106</v>
       </c>
+      <c r="H42" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="I42" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="J42" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="44" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="24"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="26"/>
     </row>
     <row r="46" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="6" t="s">
@@ -1958,14 +1973,8 @@
       <c r="E46" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H46" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="I46" s="23"/>
-      <c r="J46" s="23"/>
-      <c r="K46" s="24"/>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>21</v>
       </c>
@@ -1978,18 +1987,12 @@
       <c r="E47" s="9">
         <v>1</v>
       </c>
-      <c r="H47" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I47" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="J47" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="K47" s="13" t="s">
-        <v>25</v>
-      </c>
+      <c r="H47" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="I47" s="25"/>
+      <c r="J47" s="25"/>
+      <c r="K47" s="26"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
@@ -2004,17 +2007,17 @@
       <c r="E48" s="9">
         <v>23</v>
       </c>
-      <c r="H48" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I48" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="J48" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K48" s="9">
+      <c r="H48" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I48" s="18" t="s">
         <v>1</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K48" s="13" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
@@ -2031,7 +2034,7 @@
         <v>65</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="I49" s="11" t="s">
         <v>79</v>
@@ -2040,7 +2043,7 @@
         <v>26</v>
       </c>
       <c r="K49" s="9">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
@@ -2057,16 +2060,16 @@
         <v>66</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="J50" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K50" s="9" t="s">
-        <v>74</v>
+      <c r="K50" s="9">
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
@@ -2083,7 +2086,7 @@
         <v>39</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="I51" s="11" t="s">
         <v>52</v>
@@ -2092,7 +2095,7 @@
         <v>26</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
@@ -2109,16 +2112,16 @@
         <v>39</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I52" s="11" t="s">
         <v>52</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K52" s="9" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
@@ -2135,7 +2138,7 @@
         <v>39</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I53" s="11" t="s">
         <v>52</v>
@@ -2161,7 +2164,7 @@
         <v>68</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>96</v>
+        <v>5</v>
       </c>
       <c r="I54" s="11" t="s">
         <v>52</v>
@@ -2186,8 +2189,8 @@
       <c r="E55" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="H55" s="4" t="s">
-        <v>10</v>
+      <c r="H55" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="I55" s="11" t="s">
         <v>52</v>
@@ -2196,7 +2199,7 @@
         <v>27</v>
       </c>
       <c r="K55" s="9" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
@@ -2213,16 +2216,16 @@
         <v>70</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I56" s="11" t="s">
         <v>52</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K56" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
@@ -2239,16 +2242,16 @@
         <v>71</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>109</v>
+        <v>11</v>
       </c>
       <c r="I57" s="11" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="J57" s="11" t="s">
         <v>26</v>
       </c>
       <c r="K57" s="9" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
@@ -2265,16 +2268,16 @@
         <v>57</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J58" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K58" s="21">
-        <v>42170.75</v>
+      <c r="K58" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
@@ -2291,7 +2294,7 @@
         <v>42170.583333333336</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="I59" s="11" t="s">
         <v>80</v>
@@ -2300,14 +2303,14 @@
         <v>26</v>
       </c>
       <c r="K59" s="21">
-        <v>42170.583333333336</v>
+        <v>42170.75</v>
       </c>
     </row>
     <row r="60" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C60" s="26" t="s">
+      <c r="C60" s="23" t="s">
         <v>114</v>
       </c>
       <c r="D60" s="12" t="s">
@@ -2316,33 +2319,45 @@
       <c r="E60" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="H60" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="I60" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="J60" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K60" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H60" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I60" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="J60" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K60" s="21">
+        <v>42170.583333333336</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="19"/>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
+      <c r="H61" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="I61" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="J61" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K61" s="10" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="62" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="22" t="s">
+      <c r="B63" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="C63" s="23"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="24"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="26"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" s="6" t="s">
@@ -2530,7 +2545,7 @@
       <c r="B77" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C77" s="26" t="s">
+      <c r="C77" s="23" t="s">
         <v>114</v>
       </c>
       <c r="D77" s="12" t="s">
@@ -2548,7 +2563,7 @@
     <mergeCell ref="H34:K34"/>
     <mergeCell ref="B45:E45"/>
     <mergeCell ref="B28:E28"/>
-    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="H47:K47"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="H3:K3"/>
   </mergeCells>

</xml_diff>

<commit_message>
Update to Registry Table
RegistryID (PK)
WeddingID (FK)
</commit_message>
<xml_diff>
--- a/Wedding Builder Data Model.xlsx
+++ b/Wedding Builder Data Model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephanie\Documents\_UM Dearborn - CIS 435 Web Technology\Group Project\Data Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\435TeamProject\WeddingSiteBuilderSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="118">
   <si>
     <t>Column Name</t>
   </si>
@@ -405,7 +405,13 @@
     </r>
   </si>
   <si>
-    <t>RSVPLinkId (PK)</t>
+    <t>RSVPLinkID (PK)</t>
+  </si>
+  <si>
+    <t>RegistryID (PK)</t>
+  </si>
+  <si>
+    <t>WeddingID(FK)</t>
   </si>
 </sst>
 </file>
@@ -658,7 +664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -713,6 +719,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1003,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K77"/>
+  <dimension ref="B2:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,18 +1035,18 @@
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
-      <c r="H3" s="24" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
+      <c r="H3" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="27"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -1203,18 +1210,18 @@
       <c r="K10" s="14"/>
     </row>
     <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
-      <c r="H11" s="24" t="s">
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
+      <c r="H11" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
@@ -1607,12 +1614,12 @@
       </c>
     </row>
     <row r="28" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="27"/>
       <c r="H28" s="2" t="s">
         <v>17</v>
       </c>
@@ -1736,12 +1743,12 @@
       <c r="E34" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="24" t="s">
+      <c r="H34" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="27"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
@@ -1953,12 +1960,12 @@
     </row>
     <row r="44" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="24" t="s">
+      <c r="B45" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="27"/>
     </row>
     <row r="46" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="6" t="s">
@@ -1987,12 +1994,12 @@
       <c r="E47" s="9">
         <v>1</v>
       </c>
-      <c r="H47" s="24" t="s">
+      <c r="H47" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="I47" s="25"/>
-      <c r="J47" s="25"/>
-      <c r="K47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="27"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
@@ -2059,7 +2066,7 @@
       <c r="E50" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="H50" s="24" t="s">
         <v>63</v>
       </c>
       <c r="I50" s="11" t="s">
@@ -2352,12 +2359,12 @@
     </row>
     <row r="62" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="24" t="s">
+      <c r="B63" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="27"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" s="6" t="s">
@@ -2374,8 +2381,8 @@
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="2" t="s">
-        <v>54</v>
+      <c r="B65" s="24" t="s">
+        <v>116</v>
       </c>
       <c r="C65" s="11" t="s">
         <v>79</v>
@@ -2383,13 +2390,11 @@
       <c r="D65" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E65" s="9">
-        <v>1</v>
-      </c>
+      <c r="E65" s="9"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="2" t="s">
-        <v>83</v>
+      <c r="B66" s="24" t="s">
+        <v>117</v>
       </c>
       <c r="C66" s="11" t="s">
         <v>79</v>
@@ -2398,43 +2403,43 @@
         <v>26</v>
       </c>
       <c r="E66" s="9">
-        <v>77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="D67" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E67" s="9" t="s">
-        <v>82</v>
+      <c r="E67" s="9">
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="D69" s="11" t="s">
         <v>27</v>
@@ -2445,7 +2450,7 @@
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C70" s="11" t="s">
         <v>52</v>
@@ -2459,7 +2464,7 @@
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
-        <v>96</v>
+        <v>5</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>52</v>
@@ -2472,8 +2477,8 @@
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="4" t="s">
-        <v>10</v>
+      <c r="B72" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="C72" s="11" t="s">
         <v>52</v>
@@ -2487,71 +2492,85 @@
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C73" s="11" t="s">
         <v>52</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C75" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D74" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E74" s="9" t="s">
+      <c r="D75" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E75" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="2" t="s">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="C76" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="D75" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E75" s="15" t="s">
+      <c r="D76" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E76" s="15" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="4" t="s">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C76" s="11" t="s">
+      <c r="C77" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D76" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E76" s="21">
+      <c r="D77" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E77" s="21">
         <v>42170.583333333336</v>
       </c>
     </row>
-    <row r="77" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="5" t="s">
+    <row r="78" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C77" s="23" t="s">
+      <c r="C78" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="D77" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E77" s="10" t="s">
+      <c r="D78" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E78" s="10" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2569,7 +2588,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K27" r:id="rId1"/>
-    <hyperlink ref="E75" r:id="rId2"/>
+    <hyperlink ref="E76" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" orientation="landscape" r:id="rId3"/>

</xml_diff>